<commit_message>
Commit 57 Final Version 1.0.3.1
Sample data error & model uniwue value change
</commit_message>
<xml_diff>
--- a/Data/Lotery/01Ventas(semana11-2020).xlsx
+++ b/Data/Lotery/01Ventas(semana11-2020).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deusto-my.sharepoint.com/personal/oierajenjo_opendeusto_es/Documents/UNI/ASIGNATURAS/CURSO5/CURSO5-2/TFGII/ManagementAssistant/Data/Lotery/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Infor\Django\ManagementAssistant\Data\Lotery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="8_{C1056290-630D-4331-950B-23C30A2B39D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A5AD47FD-99B3-4BB9-930B-F2CFF6E0AFF0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E906A626-0F44-42D6-A462-1D1B285E8994}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{F0A51790-6436-4E29-9921-8F400FED1FD6}"/>
+    <workbookView xWindow="-22320" yWindow="3450" windowWidth="21600" windowHeight="11385" xr2:uid="{F0A51790-6436-4E29-9921-8F400FED1FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="56">
   <si>
     <t>Día</t>
   </si>
@@ -183,6 +183,24 @@
   </si>
   <si>
     <t>45,00</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>151,00</t>
+  </si>
+  <si>
+    <t>13,00</t>
+  </si>
+  <si>
+    <t>120,00</t>
+  </si>
+  <si>
+    <t>141,00</t>
+  </si>
+  <si>
+    <t>137,50</t>
   </si>
 </sst>
 </file>
@@ -564,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727546D4-E49F-4187-B10D-AB256E21EE17}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1419,45 +1437,129 @@
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
+      <c r="A41" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="2">
+        <v>151</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
+      <c r="A42" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="2">
+        <v>13</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
+      <c r="A43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" s="2">
+        <v>240</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
+      <c r="A44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="2">
+        <v>94</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="G44" s="2"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
+      <c r="A45" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="2">
+        <v>55</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
+      <c r="A46" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="2">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="G46" s="2"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1502,21 +1604,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000A348C43CAE06B48B5DC43CBEFA70751" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="31eafd6b2a33a82afe242ab92e22c5c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dd4158fc-877b-4374-8360-f1428db8a505" xmlns:ns4="0da9a98f-4f32-486d-97d0-1848353fd73b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="58e6caaeaae4ab5063b7057fce553289" ns3:_="" ns4:_="">
     <xsd:import namespace="dd4158fc-877b-4374-8360-f1428db8a505"/>
@@ -1725,24 +1812,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79C1A85C-297D-4678-8B10-3ED0DA0130C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F16FFE3-0D65-48F2-8BD3-4FF8406DEE91}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E296B69-F6E4-4FA3-BB16-19EF72E232AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1759,4 +1844,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F16FFE3-0D65-48F2-8BD3-4FF8406DEE91}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79C1A85C-297D-4678-8B10-3ED0DA0130C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>